<commit_message>
data van de loadtest
</commit_message>
<xml_diff>
--- a/Locust/DATA/test instellingen.xlsx
+++ b/Locust/DATA/test instellingen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jim\Documents\GitHub\DE-group-5\Locust\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C2B481-C7AB-4D6F-82BE-2C7499F72555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78E9D15-8BA1-453A-B265-78CEC6365F3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4395" yWindow="3105" windowWidth="21600" windowHeight="11385" xr2:uid="{1010000A-E7AA-4CBC-B333-59ACFC71CF6C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>LOAD TEST</t>
   </si>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D5D2D9-418F-47FB-B0B9-0D02305F3834}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,12 +440,12 @@
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -453,7 +453,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -466,8 +466,20 @@
       <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -483,8 +495,20 @@
       <c r="E4">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <v>20</v>
+      </c>
+      <c r="J4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -500,8 +524,20 @@
       <c r="E5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -517,8 +553,20 @@
       <c r="E6">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="I6">
+        <v>100</v>
+      </c>
+      <c r="J6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -534,8 +582,20 @@
       <c r="E7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -551,8 +611,20 @@
       <c r="E8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>1000</v>
+      </c>
+      <c r="H8">
+        <v>1000</v>
+      </c>
+      <c r="I8">
+        <v>1000</v>
+      </c>
+      <c r="J8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -566,6 +638,18 @@
         <v>20</v>
       </c>
       <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <v>20</v>
+      </c>
+      <c r="H9">
+        <v>20</v>
+      </c>
+      <c r="I9">
+        <v>20</v>
+      </c>
+      <c r="J9">
         <v>20</v>
       </c>
     </row>

</xml_diff>